<commit_message>
membuat tabel penetapan simpanan dan simpanan khusus
</commit_message>
<xml_diff>
--- a/database/data/demoMember.xlsx
+++ b/database/data/demoMember.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek Sekolah\koperasi-api\database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2391B3-53EB-4358-BC80-CEE335B4D12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A402F382-79AE-4836-81BD-09D1457B2C82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{546E153C-1E86-49B4-B568-B2B006966278}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{546E153C-1E86-49B4-B568-B2B006966278}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
   <si>
     <t>name</t>
   </si>
@@ -490,6 +481,18 @@
   </si>
   <si>
     <t>astri@gmail.com</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>pns</t>
+  </si>
+  <si>
+    <t>p3k</t>
+  </si>
+  <si>
+    <t>cpns</t>
   </si>
 </sst>
 </file>
@@ -930,25 +933,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952E8104-37F1-403A-B6FC-BA3C418C2637}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I21" sqref="I21:I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,8 +977,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -999,8 +1006,11 @@
       <c r="H2" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1025,8 +1035,11 @@
       <c r="H3" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1051,8 +1064,11 @@
       <c r="H4" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1077,8 +1093,11 @@
       <c r="H5" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -1103,8 +1122,11 @@
       <c r="H6" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -1129,8 +1151,11 @@
       <c r="H7" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1155,8 +1180,11 @@
       <c r="H8" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1181,8 +1209,11 @@
       <c r="H9" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1207,8 +1238,11 @@
       <c r="H10" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1233,8 +1267,11 @@
       <c r="H11" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1259,8 +1296,11 @@
       <c r="H12" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1285,8 +1325,11 @@
       <c r="H13" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -1311,8 +1354,11 @@
       <c r="H14" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1337,8 +1383,11 @@
       <c r="H15" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1363,8 +1412,11 @@
       <c r="H16" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1389,8 +1441,11 @@
       <c r="H17" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1415,8 +1470,11 @@
       <c r="H18" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1441,8 +1499,11 @@
       <c r="H19" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1467,8 +1528,11 @@
       <c r="H20" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1493,8 +1557,11 @@
       <c r="H21" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -1519,8 +1586,11 @@
       <c r="H22" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1545,8 +1615,11 @@
       <c r="H23" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1571,8 +1644,11 @@
       <c r="H24" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -1597,8 +1673,11 @@
       <c r="H25" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -1623,8 +1702,11 @@
       <c r="H26" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -1649,8 +1731,11 @@
       <c r="H27" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1675,8 +1760,11 @@
       <c r="H28" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>46</v>
       </c>
@@ -1700,6 +1788,9 @@
       </c>
       <c r="H29" s="1" t="s">
         <v>150</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memperbarui sistem role dan membuat beberapa crud api seperti kategori, sub-kategori, produk, dan barang
</commit_message>
<xml_diff>
--- a/database/data/demoMember.xlsx
+++ b/database/data/demoMember.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A402F382-79AE-4836-81BD-09D1457B2C82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C09B44F-854D-42AC-AE5D-E5FFA67DC3E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{546E153C-1E86-49B4-B568-B2B006966278}"/>
   </bookViews>
@@ -936,7 +936,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:I29"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix: memperbaiki struktur tabel invoices dan members
</commit_message>
<xml_diff>
--- a/database/data/demoMember.xlsx
+++ b/database/data/demoMember.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE21790F-D561-4F0D-9FAD-63A2FEF12E9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20445CA8-840D-469D-BB5F-3E2ADAF88660}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{546E153C-1E86-49B4-B568-B2B006966278}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="160">
   <si>
     <t>name</t>
   </si>
@@ -493,6 +493,18 @@
   </si>
   <si>
     <t>cpns</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>PNS Golongan IV</t>
+  </si>
+  <si>
+    <t>honor</t>
+  </si>
+  <si>
+    <t>PNS Golongan III</t>
   </si>
 </sst>
 </file>
@@ -933,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952E8104-37F1-403A-B6FC-BA3C418C2637}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,9 +962,10 @@
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,8 +993,11 @@
       <c r="I1" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1009,8 +1025,11 @@
       <c r="I2" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1038,8 +1057,11 @@
       <c r="I3" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1067,8 +1089,11 @@
       <c r="I4" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1094,10 +1119,13 @@
         <v>126</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="J5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
@@ -1123,10 +1151,13 @@
         <v>127</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
@@ -1154,8 +1185,11 @@
       <c r="I7" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1183,8 +1217,11 @@
       <c r="I8" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1212,8 +1249,11 @@
       <c r="I9" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1241,8 +1281,11 @@
       <c r="I10" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1270,8 +1313,11 @@
       <c r="I11" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
@@ -1299,8 +1345,11 @@
       <c r="I12" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -1328,8 +1377,11 @@
       <c r="I13" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -1357,8 +1409,11 @@
       <c r="I14" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1386,8 +1441,11 @@
       <c r="I15" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1415,8 +1473,11 @@
       <c r="I16" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1444,8 +1505,11 @@
       <c r="I17" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -1473,8 +1537,11 @@
       <c r="I18" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -1502,8 +1569,11 @@
       <c r="I19" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1531,8 +1601,11 @@
       <c r="I20" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -1560,8 +1633,11 @@
       <c r="I21" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -1589,8 +1665,11 @@
       <c r="I22" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -1618,8 +1697,11 @@
       <c r="I23" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -1647,8 +1729,11 @@
       <c r="I24" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -1676,8 +1761,11 @@
       <c r="I25" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -1705,8 +1793,11 @@
       <c r="I26" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -1734,8 +1825,11 @@
       <c r="I27" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1763,8 +1857,11 @@
       <c r="I28" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>46</v>
       </c>
@@ -1791,6 +1888,9 @@
       </c>
       <c r="I29" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: response api pada dashboard anggota
</commit_message>
<xml_diff>
--- a/database/data/demoMember.xlsx
+++ b/database/data/demoMember.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\technoG\latest\koperasi-api\database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\techG\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB6A921-57DF-484F-805A-25D874F636CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA84680-295C-4EFA-A88B-CBDD6202AF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -509,7 +522,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,6 +566,13 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -621,11 +641,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -650,14 +671,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -928,27 +953,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="26" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -983,7 +1008,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1041,7 @@
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1049,7 +1074,7 @@
       </c>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1082,7 +1107,7 @@
       </c>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1115,7 +1140,7 @@
       </c>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1148,7 +1173,7 @@
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1181,7 +1206,7 @@
       </c>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1214,7 +1239,7 @@
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -1247,7 +1272,7 @@
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -1280,7 +1305,7 @@
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1313,7 +1338,7 @@
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1346,7 +1371,7 @@
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>75</v>
       </c>
@@ -1379,7 +1404,7 @@
       </c>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>80</v>
       </c>
@@ -1412,7 +1437,7 @@
       </c>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
@@ -1445,7 +1470,7 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -1478,7 +1503,7 @@
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>95</v>
       </c>
@@ -1511,7 +1536,7 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -1544,7 +1569,7 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>105</v>
       </c>
@@ -1577,7 +1602,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>110</v>
       </c>
@@ -1610,7 +1635,7 @@
       </c>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>115</v>
       </c>
@@ -1643,7 +1668,7 @@
       </c>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>120</v>
       </c>
@@ -1676,7 +1701,7 @@
       </c>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>125</v>
       </c>
@@ -1709,7 +1734,7 @@
       </c>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>130</v>
       </c>
@@ -1742,7 +1767,7 @@
       </c>
       <c r="K24" s="9"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>135</v>
       </c>
@@ -1775,7 +1800,7 @@
       </c>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>140</v>
       </c>
@@ -1808,7 +1833,7 @@
       </c>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>145</v>
       </c>
@@ -1841,11 +1866,11 @@
       </c>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="11" t="s">
         <v>151</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -1874,7 +1899,7 @@
       </c>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>155</v>
       </c>
@@ -1907,977 +1932,977 @@
       </c>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
add: trait soft delete pada model; response api untuk simpanan dan pinjaman member
</commit_message>
<xml_diff>
--- a/database/data/demoMember.xlsx
+++ b/database/data/demoMember.xlsx
@@ -1,34 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\techG\koperasi-api\database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMKN 1 Cianjur\Documents\technoG\koperasi\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA84680-295C-4EFA-A88B-CBDD6202AF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC735DE3-C139-4193-B1E4-C1AF4FEA118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -329,9 +316,6 @@
     <t>089273485234</t>
   </si>
   <si>
-    <t>intang</t>
-  </si>
-  <si>
     <t>12345693</t>
   </si>
   <si>
@@ -516,6 +500,9 @@
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -953,27 +940,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="26" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1005,10 +992,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1041,7 +1028,7 @@
       </c>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -1074,7 +1061,7 @@
       </c>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1094,7 @@
       </c>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1140,7 +1127,7 @@
       </c>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1173,7 +1160,7 @@
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -1206,7 +1193,7 @@
       </c>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1239,7 +1226,7 @@
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -1272,7 +1259,7 @@
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -1305,7 +1292,7 @@
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1338,7 +1325,7 @@
       </c>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1371,7 +1358,7 @@
       </c>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>75</v>
       </c>
@@ -1404,7 +1391,7 @@
       </c>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>80</v>
       </c>
@@ -1437,7 +1424,7 @@
       </c>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
@@ -1470,7 +1457,7 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -1503,7 +1490,7 @@
       </c>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>95</v>
       </c>
@@ -1523,10 +1510,10 @@
         <v>15</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>36</v>
@@ -1536,18 +1523,18 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>23</v>
@@ -1556,10 +1543,10 @@
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>36</v>
@@ -1569,18 +1556,18 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>106</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>23</v>
@@ -1589,10 +1576,10 @@
         <v>15</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>36</v>
@@ -1602,18 +1589,18 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>110</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>111</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>23</v>
@@ -1622,10 +1609,10 @@
         <v>15</v>
       </c>
       <c r="G20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>36</v>
@@ -1635,18 +1622,18 @@
       </c>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>23</v>
@@ -1655,10 +1642,10 @@
         <v>15</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>42</v>
@@ -1668,18 +1655,18 @@
       </c>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>23</v>
@@ -1688,10 +1675,10 @@
         <v>15</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>42</v>
@@ -1701,18 +1688,18 @@
       </c>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>14</v>
@@ -1721,10 +1708,10 @@
         <v>15</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>42</v>
@@ -1734,18 +1721,18 @@
       </c>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>14</v>
@@ -1754,10 +1741,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>42</v>
@@ -1767,18 +1754,18 @@
       </c>
       <c r="K24" s="9"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>136</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>23</v>
@@ -1787,10 +1774,10 @@
         <v>15</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>42</v>
@@ -1800,18 +1787,18 @@
       </c>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>14</v>
@@ -1820,10 +1807,10 @@
         <v>15</v>
       </c>
       <c r="G26" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>42</v>
@@ -1833,18 +1820,18 @@
       </c>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>23</v>
@@ -1853,10 +1840,10 @@
         <v>15</v>
       </c>
       <c r="G27" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>42</v>
@@ -1866,18 +1853,18 @@
       </c>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>150</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>151</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>14</v>
@@ -1886,10 +1873,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>42</v>
@@ -1899,18 +1886,18 @@
       </c>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>14</v>
@@ -1919,10 +1906,10 @@
         <v>15</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="I29" s="7" t="s">
         <v>42</v>
@@ -1932,977 +1919,977 @@
       </c>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>